<commit_message>
Export and import same file for same result
</commit_message>
<xml_diff>
--- a/test/fixtures/files/TestGenericTemplate.xlsx
+++ b/test/fixtures/files/TestGenericTemplate.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewg/projects/SDP-Vocabulary-Service/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apellitieri/Desktop/CDC/SDP-Vocabulary-Service/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EBD933-0B05-9D4D-8327-2FFEC21C7747}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21640" yWindow="3840" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3840" windowWidth="25600" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="8" r:id="rId1"/>
+    <sheet name="Survey Questions" sheetId="8" r:id="rId1"/>
     <sheet name="RS Activate Deactivate Flag" sheetId="4" r:id="rId2"/>
     <sheet name="RS Communication Doc Type" sheetId="9" r:id="rId3"/>
+    <sheet name="Tag 1" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="100">
   <si>
     <t>Response Set Name</t>
   </si>
@@ -55,18 +57,6 @@
     <t>Question Response Type (R)</t>
   </si>
   <si>
-    <t>Question Tag Name (O)</t>
-  </si>
-  <si>
-    <t>Question Tag Value (O)</t>
-  </si>
-  <si>
-    <t>Question Code System Identifier (O)</t>
-  </si>
-  <si>
-    <t>Response Set Name (C)</t>
-  </si>
-  <si>
     <t>Response Set Source (C)</t>
   </si>
   <si>
@@ -311,13 +301,46 @@
   </si>
   <si>
     <t>https://phinvads.cdc.gov/vads/ViewValueSet.action?oid=2.16.840.1.113883.6.90</t>
+  </si>
+  <si>
+    <t>Question Tag Table (O)</t>
+  </si>
+  <si>
+    <t>Tag 1</t>
+  </si>
+  <si>
+    <t>Tag Name (R)</t>
+  </si>
+  <si>
+    <t>Tag Value (R)</t>
+  </si>
+  <si>
+    <t>Code System Identifier (O)</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Something</t>
+  </si>
+  <si>
+    <t>Else</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Local Response Set Table (C)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,7 +392,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,6 +465,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -519,9 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -662,6 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -981,29 +1008,27 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:K210"/>
+  <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.83203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="35.5" style="5" customWidth="1"/>
     <col min="6" max="7" width="13.33203125" style="5" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13" style="5" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="5"/>
+    <col min="9" max="9" width="29.6640625" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:9" ht="45.5" customHeight="1">
+      <c r="A1" s="62" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -1013,10 +1038,10 @@
         <v>6</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>2</v>
@@ -1025,1503 +1050,1447 @@
         <v>5</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="56" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="58"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-    </row>
-    <row r="3" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+    <row r="2" spans="1:9" s="55" customFormat="1">
+      <c r="A2" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="57"/>
+      <c r="H2" s="60"/>
+    </row>
+    <row r="3" spans="1:9" s="37" customFormat="1">
+      <c r="A3" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="35"/>
+      <c r="H3" s="30"/>
+    </row>
+    <row r="4" spans="1:9" s="34" customFormat="1">
+      <c r="A4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="F4" s="32"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" s="63" customFormat="1" ht="30">
+      <c r="A5" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="69"/>
+    </row>
+    <row r="6" spans="1:9" s="63" customFormat="1" ht="30">
+      <c r="A6" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="36"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-    </row>
-    <row r="4" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="B6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="F4" s="33"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="68" t="s">
+      <c r="C6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="68"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
+    </row>
+    <row r="7" spans="1:9" s="63" customFormat="1" ht="30">
+      <c r="A7" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="68"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="74" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" s="26" t="s">
+      <c r="H7" s="68"/>
+      <c r="I7" s="69"/>
+    </row>
+    <row r="8" spans="1:9" s="63" customFormat="1" ht="30">
+      <c r="A8" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="68"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="68"/>
+      <c r="I8" s="69"/>
+    </row>
+    <row r="9" spans="1:9" s="63" customFormat="1" ht="30">
+      <c r="A9" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="68"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
+    </row>
+    <row r="10" spans="1:9" s="63" customFormat="1" ht="30">
+      <c r="A10" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="68"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="68"/>
+      <c r="I10" s="69"/>
+    </row>
+    <row r="11" spans="1:9" s="63" customFormat="1" ht="30">
+      <c r="A11" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="68"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="68"/>
+      <c r="I11" s="69"/>
+    </row>
+    <row r="12" spans="1:9" s="34" customFormat="1">
+      <c r="A12" s="26" t="s">
         <v>35</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="70"/>
-    </row>
-    <row r="6" spans="1:11" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="70"/>
-    </row>
-    <row r="7" spans="1:11" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="70"/>
-    </row>
-    <row r="8" spans="1:11" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="69"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="70"/>
-    </row>
-    <row r="9" spans="1:11" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="68" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="70"/>
-    </row>
-    <row r="10" spans="1:11" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="69"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="70"/>
-    </row>
-    <row r="11" spans="1:11" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="69"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="70"/>
-    </row>
-    <row r="12" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
-        <v>39</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="33"/>
+      <c r="F12" s="32"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
-        <v>38</v>
+    </row>
+    <row r="13" spans="1:9" s="34" customFormat="1">
+      <c r="A13" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="33"/>
+      <c r="F13" s="32"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="68" t="s">
+    </row>
+    <row r="14" spans="1:9" ht="30">
+      <c r="A14" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="68"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="70"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:9" ht="30">
+      <c r="A15" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="68"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="70"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" ht="30">
+      <c r="A16" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B16" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="69"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="71"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="14"/>
-    </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="68" t="s">
+      <c r="C16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="68"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="70"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="1:9" ht="30">
+      <c r="A17" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B17" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="69"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="71"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="68" t="s">
+      <c r="C17" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="68"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="70"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" ht="30">
+      <c r="A18" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B18" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="69"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="71"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="68" t="s">
+      <c r="C18" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="68"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="1:9" ht="30">
+      <c r="A19" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B19" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="69"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="71"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="68" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="69"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
-    </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>51</v>
-      </c>
       <c r="C19" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="69"/>
+        <v>29</v>
+      </c>
+      <c r="D19" s="68"/>
       <c r="E19" s="17"/>
-      <c r="F19" s="26" t="s">
-        <v>35</v>
+      <c r="F19" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-    </row>
-    <row r="20" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
+    </row>
+    <row r="20" spans="1:9" s="34" customFormat="1">
+      <c r="A20" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="9"/>
+      <c r="F20" s="32"/>
+    </row>
+    <row r="21" spans="1:9" s="37" customFormat="1">
+      <c r="A21" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="30"/>
+      <c r="F21" s="35"/>
+    </row>
+    <row r="22" spans="1:9" s="42" customFormat="1">
+      <c r="A22" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="9"/>
-      <c r="F20" s="33"/>
-    </row>
-    <row r="21" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="31"/>
-      <c r="F21" s="36"/>
-    </row>
-    <row r="22" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="39" t="s">
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41"/>
+      <c r="F22" s="39"/>
+    </row>
+    <row r="23" spans="1:9" s="45" customFormat="1">
+      <c r="A23" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="46"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="28"/>
+      <c r="F23" s="43"/>
+    </row>
+    <row r="24" spans="1:9" ht="30">
+      <c r="A24" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
-      <c r="F22" s="40"/>
-    </row>
-    <row r="23" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="29"/>
-      <c r="F23" s="44"/>
-    </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="68" t="s">
-        <v>61</v>
-      </c>
       <c r="B24" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="69"/>
+        <v>29</v>
+      </c>
+      <c r="D24" s="68"/>
       <c r="E24" s="17"/>
-      <c r="F24" s="26" t="s">
-        <v>35</v>
+      <c r="F24" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-    </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="68" t="s">
-        <v>63</v>
+    </row>
+    <row r="25" spans="1:9" ht="30">
+      <c r="A25" s="67" t="s">
+        <v>59</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="69"/>
+        <v>29</v>
+      </c>
+      <c r="D25" s="68"/>
       <c r="E25" s="17"/>
-      <c r="F25" s="26" t="s">
-        <v>35</v>
+      <c r="F25" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-    </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="68" t="s">
-        <v>65</v>
+    </row>
+    <row r="26" spans="1:9" ht="30">
+      <c r="A26" s="67" t="s">
+        <v>61</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="69"/>
+        <v>29</v>
+      </c>
+      <c r="D26" s="68"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="26" t="s">
-        <v>35</v>
+      <c r="F26" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-    </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A27" s="68" t="s">
-        <v>67</v>
+    </row>
+    <row r="27" spans="1:9" ht="30">
+      <c r="A27" s="67" t="s">
+        <v>63</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="69"/>
+        <v>29</v>
+      </c>
+      <c r="D27" s="68"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="26" t="s">
-        <v>35</v>
+      <c r="F27" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-    </row>
-    <row r="28" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="29"/>
-      <c r="F28" s="44"/>
-    </row>
-    <row r="29" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
-      <c r="F29" s="40"/>
-    </row>
-    <row r="30" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="51"/>
-      <c r="F30" s="59"/>
-    </row>
-    <row r="31" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="55"/>
-      <c r="F31" s="65"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="72" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="F32" s="26"/>
+    </row>
+    <row r="28" spans="1:9" s="45" customFormat="1">
+      <c r="A28" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="28"/>
+      <c r="F28" s="43"/>
+    </row>
+    <row r="29" spans="1:9" s="42" customFormat="1">
+      <c r="A29" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="40"/>
+      <c r="D29" s="41"/>
+      <c r="F29" s="39"/>
+    </row>
+    <row r="30" spans="1:9" s="48" customFormat="1">
+      <c r="A30" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
+      <c r="F30" s="58"/>
+    </row>
+    <row r="31" spans="1:9" s="52" customFormat="1">
+      <c r="A31" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="53"/>
+      <c r="D31" s="54"/>
+      <c r="F31" s="64"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="25"/>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-    </row>
-    <row r="33" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A33" s="72" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F33" s="26"/>
+    </row>
+    <row r="33" spans="1:9" ht="42">
+      <c r="A33" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F33" s="25"/>
       <c r="G33" s="17"/>
       <c r="H33" s="17"/>
       <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="23"/>
-      <c r="F34" s="26"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="17"/>
       <c r="H34" s="17"/>
       <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-    </row>
-    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="73" t="s">
-        <v>80</v>
-      </c>
-      <c r="F35" s="26"/>
+    </row>
+    <row r="35" spans="1:9" ht="30">
+      <c r="A35" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="72" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="25"/>
       <c r="G35" s="17"/>
       <c r="H35" s="17"/>
       <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-    </row>
-    <row r="36" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="54"/>
-      <c r="F36" s="65"/>
-    </row>
-    <row r="37" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="50"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-    </row>
-    <row r="38" spans="1:11" s="56" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="57"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:9" s="52" customFormat="1">
+      <c r="A36" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="53"/>
+      <c r="F36" s="64"/>
+    </row>
+    <row r="37" spans="1:9" s="48" customFormat="1">
+      <c r="A37" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="49"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+    </row>
+    <row r="38" spans="1:9" s="55" customFormat="1">
+      <c r="A38" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="56"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+    </row>
+    <row r="39" spans="1:9">
       <c r="C39" s="3"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="C40" s="3"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="C41" s="3"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="C42" s="3"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="C43" s="3"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="C44" s="3"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="C45" s="3"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="C46" s="3"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="C47" s="3"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="C48" s="3"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:7">
       <c r="C49" s="3"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:7">
       <c r="C50" s="3"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:7">
       <c r="C51" s="3"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:7">
       <c r="C52" s="3"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:7">
       <c r="C53" s="3"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:7">
       <c r="C54" s="3"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:7">
       <c r="C55" s="3"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:7">
       <c r="C56" s="3"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:7">
       <c r="C57" s="3"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:7">
       <c r="C58" s="3"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:7">
       <c r="C59" s="3"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:7">
       <c r="C60" s="3"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:7">
       <c r="C61" s="3"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:7">
       <c r="C62" s="3"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:7">
       <c r="C63" s="3"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:7">
       <c r="C64" s="3"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:7">
       <c r="C65" s="3"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:7">
       <c r="C66" s="3"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:7">
       <c r="C67" s="3"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:7">
       <c r="C68" s="3"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:7">
       <c r="C69" s="3"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:7">
       <c r="C70" s="3"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:7">
       <c r="C71" s="3"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:7">
       <c r="C72" s="3"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:7">
       <c r="C73" s="3"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:7">
       <c r="C74" s="3"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:7">
       <c r="C75" s="3"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:7">
       <c r="C76" s="3"/>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:7">
       <c r="C77" s="3"/>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:7">
       <c r="C78" s="3"/>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:7">
       <c r="C79" s="3"/>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:7">
       <c r="C80" s="3"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:7">
       <c r="C81" s="3"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:7">
       <c r="C82" s="3"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:7">
       <c r="C83" s="3"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:7">
       <c r="C84" s="3"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:7">
       <c r="C85" s="3"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:7">
       <c r="C86" s="3"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:7">
       <c r="C87" s="3"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:7">
       <c r="C88" s="3"/>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:7">
       <c r="C89" s="3"/>
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="3:7">
       <c r="C90" s="3"/>
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:7">
       <c r="C91" s="3"/>
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:7">
       <c r="C92" s="3"/>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:7">
       <c r="C93" s="3"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="3:7">
       <c r="C94" s="3"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="3:7">
       <c r="C95" s="3"/>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="3:7">
       <c r="C96" s="3"/>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
     </row>
-    <row r="97" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:7">
       <c r="C97" s="3"/>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
     </row>
-    <row r="98" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:7">
       <c r="C98" s="3"/>
       <c r="F98" s="4"/>
       <c r="G98" s="4"/>
     </row>
-    <row r="99" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:7">
       <c r="C99" s="3"/>
       <c r="F99" s="4"/>
       <c r="G99" s="4"/>
     </row>
-    <row r="100" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:7">
       <c r="C100" s="3"/>
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
     </row>
-    <row r="101" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:7">
       <c r="C101" s="3"/>
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
     </row>
-    <row r="102" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:7">
       <c r="C102" s="3"/>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
     </row>
-    <row r="103" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:7">
       <c r="C103" s="3"/>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
     </row>
-    <row r="104" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:7">
       <c r="C104" s="3"/>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
     </row>
-    <row r="105" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:7">
       <c r="C105" s="3"/>
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
     </row>
-    <row r="106" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:7">
       <c r="C106" s="3"/>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
     </row>
-    <row r="107" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:7">
       <c r="C107" s="3"/>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
     </row>
-    <row r="108" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:7">
       <c r="C108" s="3"/>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
     </row>
-    <row r="109" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:7">
       <c r="C109" s="3"/>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
     </row>
-    <row r="110" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="3:7">
       <c r="C110" s="3"/>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
     </row>
-    <row r="111" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="3:7">
       <c r="C111" s="3"/>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
     </row>
-    <row r="112" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:7">
       <c r="C112" s="3"/>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
     </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:7">
       <c r="C113" s="3"/>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
     </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:7">
       <c r="C114" s="3"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
     </row>
-    <row r="115" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:7">
       <c r="C115" s="3"/>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
     </row>
-    <row r="116" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:7">
       <c r="C116" s="3"/>
       <c r="F116" s="4"/>
       <c r="G116" s="4"/>
     </row>
-    <row r="117" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:7">
       <c r="C117" s="3"/>
       <c r="F117" s="4"/>
       <c r="G117" s="4"/>
     </row>
-    <row r="118" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:7">
       <c r="C118" s="3"/>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
     </row>
-    <row r="119" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:7">
       <c r="C119" s="3"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
     </row>
-    <row r="120" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:7">
       <c r="C120" s="3"/>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
     </row>
-    <row r="121" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:7">
       <c r="C121" s="3"/>
       <c r="F121" s="4"/>
       <c r="G121" s="4"/>
     </row>
-    <row r="122" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="3:7">
       <c r="C122" s="3"/>
       <c r="F122" s="4"/>
       <c r="G122" s="4"/>
     </row>
-    <row r="123" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:7">
       <c r="C123" s="3"/>
       <c r="F123" s="4"/>
       <c r="G123" s="4"/>
     </row>
-    <row r="124" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:7">
       <c r="C124" s="3"/>
       <c r="F124" s="4"/>
       <c r="G124" s="4"/>
     </row>
-    <row r="125" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:7">
       <c r="C125" s="3"/>
       <c r="F125" s="4"/>
       <c r="G125" s="4"/>
     </row>
-    <row r="126" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="3:7">
       <c r="C126" s="3"/>
       <c r="F126" s="4"/>
       <c r="G126" s="4"/>
     </row>
-    <row r="127" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="3:7">
       <c r="C127" s="3"/>
       <c r="F127" s="4"/>
       <c r="G127" s="4"/>
     </row>
-    <row r="128" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="3:7">
       <c r="C128" s="3"/>
       <c r="F128" s="4"/>
       <c r="G128" s="4"/>
     </row>
-    <row r="129" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:7">
       <c r="C129" s="3"/>
       <c r="F129" s="4"/>
       <c r="G129" s="4"/>
     </row>
-    <row r="130" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:7">
       <c r="C130" s="3"/>
       <c r="F130" s="4"/>
       <c r="G130" s="4"/>
     </row>
-    <row r="131" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:7">
       <c r="C131" s="3"/>
       <c r="F131" s="4"/>
       <c r="G131" s="4"/>
     </row>
-    <row r="132" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:7">
       <c r="C132" s="3"/>
       <c r="F132" s="4"/>
       <c r="G132" s="4"/>
     </row>
-    <row r="133" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:7">
       <c r="C133" s="3"/>
       <c r="F133" s="4"/>
       <c r="G133" s="4"/>
     </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:7">
       <c r="C134" s="3"/>
       <c r="F134" s="4"/>
       <c r="G134" s="4"/>
     </row>
-    <row r="135" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:7">
       <c r="C135" s="3"/>
       <c r="F135" s="4"/>
       <c r="G135" s="4"/>
     </row>
-    <row r="136" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:7">
       <c r="C136" s="3"/>
       <c r="F136" s="4"/>
       <c r="G136" s="4"/>
     </row>
-    <row r="137" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:7">
       <c r="C137" s="3"/>
       <c r="F137" s="4"/>
       <c r="G137" s="4"/>
     </row>
-    <row r="138" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:7">
       <c r="C138" s="3"/>
       <c r="F138" s="4"/>
       <c r="G138" s="4"/>
     </row>
-    <row r="139" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:7">
       <c r="C139" s="3"/>
       <c r="F139" s="4"/>
       <c r="G139" s="4"/>
     </row>
-    <row r="140" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:7">
       <c r="C140" s="3"/>
       <c r="F140" s="4"/>
       <c r="G140" s="4"/>
     </row>
-    <row r="141" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:7">
       <c r="C141" s="3"/>
       <c r="F141" s="4"/>
       <c r="G141" s="4"/>
     </row>
-    <row r="142" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:7">
       <c r="C142" s="3"/>
       <c r="F142" s="4"/>
       <c r="G142" s="4"/>
     </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:7">
       <c r="C143" s="3"/>
       <c r="F143" s="4"/>
       <c r="G143" s="4"/>
     </row>
-    <row r="144" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:7">
       <c r="C144" s="3"/>
       <c r="F144" s="4"/>
       <c r="G144" s="4"/>
     </row>
-    <row r="145" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:7">
       <c r="C145" s="3"/>
       <c r="F145" s="4"/>
       <c r="G145" s="4"/>
     </row>
-    <row r="146" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:7">
       <c r="C146" s="3"/>
       <c r="F146" s="4"/>
       <c r="G146" s="4"/>
     </row>
-    <row r="147" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:7">
       <c r="C147" s="3"/>
       <c r="F147" s="4"/>
       <c r="G147" s="4"/>
     </row>
-    <row r="148" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:7">
       <c r="C148" s="3"/>
       <c r="F148" s="4"/>
       <c r="G148" s="4"/>
     </row>
-    <row r="149" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:7">
       <c r="C149" s="3"/>
       <c r="F149" s="4"/>
       <c r="G149" s="4"/>
     </row>
-    <row r="150" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:7">
       <c r="C150" s="3"/>
       <c r="F150" s="4"/>
       <c r="G150" s="4"/>
     </row>
-    <row r="151" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:7">
       <c r="C151" s="3"/>
       <c r="F151" s="4"/>
       <c r="G151" s="4"/>
     </row>
-    <row r="152" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:7">
       <c r="C152" s="3"/>
       <c r="F152" s="4"/>
       <c r="G152" s="4"/>
     </row>
-    <row r="153" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:7">
       <c r="C153" s="3"/>
       <c r="F153" s="4"/>
       <c r="G153" s="4"/>
     </row>
-    <row r="154" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:7">
       <c r="C154" s="3"/>
       <c r="F154" s="4"/>
       <c r="G154" s="4"/>
     </row>
-    <row r="155" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:7">
       <c r="C155" s="3"/>
       <c r="F155" s="4"/>
       <c r="G155" s="4"/>
     </row>
-    <row r="156" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:7">
       <c r="C156" s="3"/>
       <c r="F156" s="4"/>
       <c r="G156" s="4"/>
     </row>
-    <row r="157" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:7">
       <c r="C157" s="3"/>
       <c r="F157" s="4"/>
       <c r="G157" s="4"/>
     </row>
-    <row r="158" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:7">
       <c r="C158" s="3"/>
       <c r="F158" s="4"/>
       <c r="G158" s="4"/>
     </row>
-    <row r="159" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:7">
       <c r="C159" s="3"/>
       <c r="F159" s="4"/>
       <c r="G159" s="4"/>
     </row>
-    <row r="160" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:7">
       <c r="C160" s="3"/>
       <c r="F160" s="4"/>
       <c r="G160" s="4"/>
     </row>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="3:7">
       <c r="C161" s="3"/>
       <c r="F161" s="4"/>
       <c r="G161" s="4"/>
     </row>
-    <row r="162" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="3:7">
       <c r="C162" s="3"/>
       <c r="F162" s="4"/>
       <c r="G162" s="4"/>
     </row>
-    <row r="163" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="3:7">
       <c r="C163" s="3"/>
       <c r="F163" s="4"/>
       <c r="G163" s="4"/>
     </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="3:7">
       <c r="C164" s="3"/>
       <c r="F164" s="4"/>
       <c r="G164" s="4"/>
     </row>
-    <row r="165" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:7">
       <c r="C165" s="3"/>
       <c r="F165" s="4"/>
       <c r="G165" s="4"/>
     </row>
-    <row r="166" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:7">
       <c r="C166" s="3"/>
       <c r="F166" s="4"/>
       <c r="G166" s="4"/>
     </row>
-    <row r="167" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:7">
       <c r="C167" s="3"/>
       <c r="F167" s="4"/>
       <c r="G167" s="4"/>
     </row>
-    <row r="168" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:7">
       <c r="C168" s="3"/>
       <c r="F168" s="4"/>
       <c r="G168" s="4"/>
     </row>
-    <row r="169" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:7">
       <c r="C169" s="3"/>
       <c r="F169" s="4"/>
       <c r="G169" s="4"/>
     </row>
-    <row r="170" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="3:7">
       <c r="C170" s="3"/>
       <c r="F170" s="4"/>
       <c r="G170" s="4"/>
     </row>
-    <row r="171" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="3:7">
       <c r="C171" s="3"/>
       <c r="F171" s="4"/>
       <c r="G171" s="4"/>
     </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="3:7">
       <c r="C172" s="3"/>
       <c r="F172" s="4"/>
       <c r="G172" s="4"/>
     </row>
-    <row r="173" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="3:7">
       <c r="C173" s="3"/>
       <c r="F173" s="4"/>
       <c r="G173" s="4"/>
     </row>
-    <row r="174" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="3:7">
       <c r="C174" s="3"/>
       <c r="F174" s="4"/>
       <c r="G174" s="4"/>
     </row>
-    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="3:7">
       <c r="C175" s="3"/>
       <c r="F175" s="4"/>
       <c r="G175" s="4"/>
     </row>
-    <row r="176" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="3:7">
       <c r="C176" s="3"/>
       <c r="F176" s="4"/>
       <c r="G176" s="4"/>
     </row>
-    <row r="177" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:7">
       <c r="C177" s="3"/>
       <c r="F177" s="4"/>
       <c r="G177" s="4"/>
     </row>
-    <row r="178" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:7">
       <c r="C178" s="3"/>
       <c r="F178" s="4"/>
       <c r="G178" s="4"/>
     </row>
-    <row r="179" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:7">
       <c r="C179" s="3"/>
       <c r="F179" s="4"/>
       <c r="G179" s="4"/>
     </row>
-    <row r="180" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:7">
       <c r="C180" s="3"/>
       <c r="F180" s="4"/>
       <c r="G180" s="4"/>
     </row>
-    <row r="181" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:7">
       <c r="C181" s="3"/>
       <c r="F181" s="4"/>
       <c r="G181" s="4"/>
     </row>
-    <row r="182" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:7">
       <c r="C182" s="3"/>
       <c r="F182" s="4"/>
       <c r="G182" s="4"/>
     </row>
-    <row r="183" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:7">
       <c r="C183" s="3"/>
       <c r="F183" s="4"/>
       <c r="G183" s="4"/>
     </row>
-    <row r="184" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:7">
       <c r="C184" s="3"/>
       <c r="F184" s="4"/>
       <c r="G184" s="4"/>
     </row>
-    <row r="185" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:7">
       <c r="C185" s="3"/>
       <c r="F185" s="4"/>
       <c r="G185" s="4"/>
     </row>
-    <row r="186" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:7">
       <c r="C186" s="3"/>
       <c r="F186" s="4"/>
       <c r="G186" s="4"/>
     </row>
-    <row r="187" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:7">
       <c r="C187" s="3"/>
       <c r="F187" s="4"/>
       <c r="G187" s="4"/>
     </row>
-    <row r="188" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="3:7">
       <c r="C188" s="3"/>
       <c r="F188" s="4"/>
       <c r="G188" s="4"/>
     </row>
-    <row r="189" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="3:7">
       <c r="C189" s="3"/>
       <c r="F189" s="4"/>
       <c r="G189" s="4"/>
     </row>
-    <row r="190" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="3:7">
       <c r="C190" s="3"/>
       <c r="F190" s="4"/>
       <c r="G190" s="4"/>
     </row>
-    <row r="191" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="3:7">
       <c r="C191" s="3"/>
       <c r="F191" s="4"/>
       <c r="G191" s="4"/>
     </row>
-    <row r="192" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="3:7">
       <c r="C192" s="3"/>
       <c r="F192" s="4"/>
       <c r="G192" s="4"/>
     </row>
-    <row r="193" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="3:7">
       <c r="C193" s="3"/>
       <c r="F193" s="4"/>
       <c r="G193" s="4"/>
     </row>
-    <row r="194" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="3:7">
       <c r="C194" s="3"/>
       <c r="F194" s="4"/>
       <c r="G194" s="4"/>
     </row>
-    <row r="195" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="3:7">
       <c r="C195" s="3"/>
       <c r="F195" s="4"/>
       <c r="G195" s="4"/>
     </row>
-    <row r="196" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="3:7">
       <c r="C196" s="3"/>
       <c r="F196" s="4"/>
       <c r="G196" s="4"/>
     </row>
-    <row r="197" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="3:7">
       <c r="C197" s="3"/>
       <c r="F197" s="4"/>
       <c r="G197" s="4"/>
     </row>
-    <row r="198" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="3:7">
       <c r="C198" s="3"/>
       <c r="F198" s="4"/>
       <c r="G198" s="4"/>
     </row>
-    <row r="199" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="3:7">
       <c r="C199" s="3"/>
       <c r="F199" s="4"/>
       <c r="G199" s="4"/>
     </row>
-    <row r="200" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="3:7">
       <c r="C200" s="3"/>
       <c r="F200" s="4"/>
       <c r="G200" s="4"/>
     </row>
-    <row r="201" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="3:7">
       <c r="C201" s="3"/>
       <c r="F201" s="4"/>
       <c r="G201" s="4"/>
     </row>
-    <row r="202" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="3:7">
       <c r="C202" s="3"/>
       <c r="F202" s="4"/>
       <c r="G202" s="4"/>
     </row>
-    <row r="203" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="3:7">
       <c r="C203" s="3"/>
       <c r="F203" s="4"/>
       <c r="G203" s="4"/>
     </row>
-    <row r="204" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="3:7">
       <c r="C204" s="3"/>
       <c r="F204" s="4"/>
       <c r="G204" s="4"/>
     </row>
-    <row r="205" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="3:7">
       <c r="C205" s="3"/>
       <c r="F205" s="4"/>
       <c r="G205" s="4"/>
     </row>
-    <row r="206" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="3:7">
       <c r="C206" s="3"/>
       <c r="F206" s="4"/>
       <c r="G206" s="4"/>
     </row>
-    <row r="207" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="3:7">
       <c r="C207" s="3"/>
       <c r="F207" s="4"/>
       <c r="G207" s="4"/>
     </row>
-    <row r="208" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="3:7">
       <c r="C208" s="3"/>
       <c r="F208" s="4"/>
       <c r="G208" s="4"/>
     </row>
-    <row r="209" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:7">
       <c r="C209" s="3"/>
       <c r="F209" s="4"/>
       <c r="G209" s="4"/>
     </row>
-    <row r="210" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:7">
       <c r="C210" s="3"/>
       <c r="F210" s="4"/>
       <c r="G210" s="4"/>
@@ -2558,7 +2527,7 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
@@ -2570,76 +2539,76 @@
     <col min="8" max="8" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
-        <v>85</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="45">
+      <c r="A2" s="66" t="s">
+        <v>81</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="5" customFormat="1">
       <c r="C3" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D3" s="7">
         <v>2</v>
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="5" customFormat="1">
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="5" customFormat="1">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="5" customFormat="1">
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="5" customFormat="1">
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="5" customFormat="1"/>
+    <row r="9" spans="1:9" s="5" customFormat="1">
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" s="5" customFormat="1"/>
+    <row r="11" spans="1:9" s="5" customFormat="1"/>
+    <row r="12" spans="1:9" s="5" customFormat="1"/>
+    <row r="13" spans="1:9" s="5" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2656,7 +2625,7 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
@@ -2668,71 +2637,122 @@
     <col min="8" max="8" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="56" x14ac:dyDescent="0.2">
-      <c r="A2" s="66" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="56">
+      <c r="A2" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="74" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1">
+      <c r="C3" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="75" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-    </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="76" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-    </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-    </row>
-    <row r="5" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1">
+      <c r="C4" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+    </row>
+    <row r="5" spans="1:9" s="5" customFormat="1">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="5" customFormat="1">
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="5" customFormat="1">
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="5" customFormat="1"/>
+    <row r="9" spans="1:9" s="5" customFormat="1">
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" s="5" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F929FC0-AC6E-6540-9F1E-EF60494A7DA1}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed issue on import of generic spreadsheet where Response Sets not created
</commit_message>
<xml_diff>
--- a/test/fixtures/files/TestGenericTemplate.xlsx
+++ b/test/fixtures/files/TestGenericTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghamilton/devel/CDC/SDPV/SDP-Vocabulary-Service/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF3F0C8-0ED2-CF4D-8C37-E82027E9FDC5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F31B52A-B535-F94C-A9CE-739BFD474CB7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30500" yWindow="-1180" windowWidth="31540" windowHeight="17360" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30240" yWindow="-4420" windowWidth="28800" windowHeight="16240" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Questions" sheetId="8" r:id="rId1"/>
@@ -3880,7 +3880,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A95" sqref="A95:XFD102"/>
+      <selection pane="bottomLeft" activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5346,7 +5346,7 @@
       <c r="A100" t="s">
         <v>160</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="59" t="s">
         <v>998</v>
       </c>
       <c r="J100" t="s">
@@ -5665,7 +5665,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed exporter to match importer
</commit_message>
<xml_diff>
--- a/test/fixtures/files/TestGenericTemplate.xlsx
+++ b/test/fixtures/files/TestGenericTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghamilton/devel/CDC/SDPV/SDP-Vocabulary-Service/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41E06E2-D1D3-D042-B86C-9B6E9ECB80BE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BAB1A1-142B-3F49-A0E7-3EB1063C550F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33480" yWindow="2600" windowWidth="25720" windowHeight="15960" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3080" yWindow="740" windowWidth="25720" windowHeight="15960" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Questions" sheetId="8" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3364" uniqueCount="1620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3365" uniqueCount="1621">
   <si>
     <t>Populate a category from the list</t>
   </si>
@@ -5030,6 +5030,9 @@
   </si>
   <si>
     <t>Code System Identifier (O)</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -5743,9 +5746,9 @@
   <dimension ref="A1:K430"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A372" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C388" sqref="C388"/>
+      <selection pane="bottomLeft" activeCell="C391" sqref="C391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11545,8 +11548,8 @@
       <c r="A388" t="s">
         <v>585</v>
       </c>
-      <c r="C388" s="63">
-        <v>8</v>
+      <c r="C388" s="63" t="s">
+        <v>1620</v>
       </c>
       <c r="J388" s="18" t="s">
         <v>586</v>

</xml_diff>